<commit_message>
load test report updatedt
</commit_message>
<xml_diff>
--- a/booking-API-Load_Stress-TestReport.xlsx
+++ b/booking-API-Load_Stress-TestReport.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\temmm\Full stack SQA_Road to SDET\assinmt\3 Load test using Jmeter\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01A555C-AFCB-4E34-A95F-B03B83F0D125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBC5671-FAEB-429E-A150-3B9323DA6A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Load-Test-Report" sheetId="1" r:id="rId1"/>
     <sheet name="Stress-Test-Report" sheetId="3" r:id="rId2"/>
-    <sheet name="dispo" sheetId="2" r:id="rId3"/>
+    <sheet name="dispo" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>Test Name</t>
   </si>
@@ -135,9 +135,6 @@
     <t>14 min</t>
   </si>
   <si>
-    <t>17 min</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Stress Test Strategy </t>
     </r>
@@ -158,10 +155,37 @@
     <t>Test-9</t>
   </si>
   <si>
+    <t>Test Step-1</t>
+  </si>
+  <si>
+    <t>Test Step-2</t>
+  </si>
+  <si>
+    <t>Test Step-3</t>
+  </si>
+  <si>
+    <t>Test Step-4</t>
+  </si>
+  <si>
+    <t>Test Step-5</t>
+  </si>
+  <si>
+    <t>Test Step-6</t>
+  </si>
+  <si>
+    <t>Test Step-7</t>
+  </si>
+  <si>
+    <t>Test Step-8</t>
+  </si>
+  <si>
+    <t>Test Step-9</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Consolas"/>
         <family val="3"/>
@@ -171,66 +195,95 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="7" tint="0.59999389629810485"/>
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> Fail </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Fail</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>in The Expected Load 2.778</t>
-    </r>
-  </si>
-  <si>
-    <t>Test Step-1</t>
-  </si>
-  <si>
-    <t>Test Step-2</t>
-  </si>
-  <si>
-    <t>Test Step-3</t>
-  </si>
-  <si>
-    <t>Test Step-4</t>
-  </si>
-  <si>
-    <t>Test Step-5</t>
-  </si>
-  <si>
-    <t>Test Step-6</t>
-  </si>
-  <si>
-    <t>Test Step-7</t>
-  </si>
-  <si>
-    <t>Test Step-8</t>
-  </si>
-  <si>
-    <t>Test Step-9</t>
-  </si>
-  <si>
+      <t>TPS:</t>
+    </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
+      <t>where the Expected Load:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">2.778 </t>
+    </r>
+  </si>
+  <si>
+    <t>16 min</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
       <t xml:space="preserve">Load Test </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="7"/>
         <rFont val="Consolas"/>
         <family val="3"/>
@@ -240,27 +293,27 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve">TPS: </t>
+      <t>TPS:</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="0"/>
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>1.638</t>
+      <t>1.984</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="7" tint="0.59999389629810485"/>
         <rFont val="Consolas"/>
         <family val="3"/>
@@ -270,7 +323,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Consolas"/>
         <family val="3"/>
@@ -280,7 +333,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="0"/>
         <rFont val="Consolas"/>
         <family val="3"/>
@@ -293,7 +346,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,46 +447,53 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="7" tint="0.59999389629810485"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="7" tint="0.59999389629810485"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
       <sz val="6"/>
-      <color theme="1"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Arial Rounded MT Bold"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="7"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,6 +562,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor rgb="FF76A5AF"/>
       </patternFill>
@@ -514,12 +580,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="5"/>
+        <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -542,23 +608,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -648,40 +703,37 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,10 +1023,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="B4:I20"/>
+  <dimension ref="B4:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G16" sqref="D16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,7 +1038,7 @@
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
@@ -996,7 +1048,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1006,7 +1058,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1096,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1062,7 +1114,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
@@ -1074,11 +1126,11 @@
       <c r="F9" s="24">
         <v>2.778</v>
       </c>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21" t="s">
@@ -1094,9 +1146,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21" t="s">
@@ -1112,9 +1164,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21" t="s">
@@ -1130,9 +1182,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="29" t="s">
@@ -1144,13 +1196,13 @@
       <c r="F13" s="29">
         <v>1667</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="35">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="21" t="s">
@@ -1162,13 +1214,13 @@
       <c r="F14" s="21">
         <v>1667</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="35">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21" t="s">
@@ -1180,13 +1232,13 @@
       <c r="F15" s="21">
         <v>1667</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="35">
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21" t="s">
@@ -1201,17 +1253,18 @@
       <c r="G16" s="40">
         <v>2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
-        <v>34</v>
-      </c>
+      <c r="H16" s="41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="19"/>
       <c r="C17" s="20"/>
       <c r="D17" s="21" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E17" s="21">
-        <v>1020</v>
+        <v>900</v>
       </c>
       <c r="F17" s="21">
         <v>1667</v>
@@ -1219,58 +1272,70 @@
       <c r="G17" s="40">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="H17" s="41">
-        <v>0.06</v>
-      </c>
-      <c r="I17" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E18" s="21">
-        <v>1200</v>
+        <v>960</v>
       </c>
       <c r="F18" s="21">
         <v>1667</v>
       </c>
-      <c r="G18" s="40">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+      <c r="G18" s="35">
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="21">
+        <v>1200</v>
+      </c>
+      <c r="F19" s="21">
+        <v>1667</v>
+      </c>
+      <c r="G19" s="35">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="25">
-        <v>1.6339999999999999</v>
-      </c>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="2:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="25">
+        <v>1.984</v>
+      </c>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="2:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1285,8 +1350,8 @@
   </sheetPr>
   <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,7 +1365,7 @@
   <sheetData>
     <row r="2" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
@@ -1386,79 +1451,70 @@
       <c r="F7" s="24">
         <v>2.778</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E8" s="21">
-        <v>1200</v>
+        <v>840</v>
       </c>
       <c r="F8" s="21">
         <v>1667</v>
       </c>
-      <c r="G8" s="38">
-        <v>8.0000000000000004E-4</v>
+      <c r="G8" s="34">
+        <v>2.0000000000000001E-4</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9" s="21">
-        <v>1200</v>
+        <v>840</v>
       </c>
       <c r="F9" s="21">
-        <v>1800</v>
-      </c>
-      <c r="G9" s="42">
-        <v>6.9999999999999999E-4</v>
-      </c>
+        <v>3000</v>
+      </c>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="21">
-        <v>1200</v>
-      </c>
-      <c r="F10" s="21">
-        <v>2200</v>
-      </c>
-      <c r="G10" s="39"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="35"/>
+      <c r="F11" s="21">
+        <v>5000</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="36"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
@@ -1473,7 +1529,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="20"/>
     </row>
@@ -1527,20 +1583,18 @@
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="25">
-        <v>1.984</v>
-      </c>
+      <c r="F21" s="25"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
+    <row r="22" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1555,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6500F655-8A29-4CAA-8550-91463AC69D29}">
-  <dimension ref="B3:E10"/>
+  <dimension ref="B3:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E10"/>
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,6 +1678,48 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="27">
+        <v>16</v>
+      </c>
+      <c r="C11" s="27">
+        <v>960</v>
+      </c>
+      <c r="D11" s="27">
+        <v>1667</v>
+      </c>
+      <c r="E11" s="28">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="21">
+        <v>960</v>
+      </c>
+      <c r="D12" s="21">
+        <v>1667</v>
+      </c>
+      <c r="E12" s="35">
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="21">
+        <v>1200</v>
+      </c>
+      <c r="D13" s="21">
+        <v>1667</v>
+      </c>
+      <c r="E13" s="35">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
stress  test report updated
</commit_message>
<xml_diff>
--- a/booking-API-Load_Stress-TestReport.xlsx
+++ b/booking-API-Load_Stress-TestReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\temmm\Full stack SQA_Road to SDET\assinmt\3 Load test using Jmeter\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBC5671-FAEB-429E-A150-3B9323DA6A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCDAD60-36E1-43BB-81C0-A1C2DAF8B575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Test Name</t>
   </si>
@@ -182,6 +182,84 @@
     <t>Test Step-9</t>
   </si>
   <si>
+    <t>16 min</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Load Test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Fail </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>TPS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1.984</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>where The Expected Load:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2.778</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -206,21 +284,11 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFC00000"/>
+        <color theme="0"/>
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>Fail</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">Lower Bottleneck: </t>
     </r>
     <r>
       <rPr>
@@ -230,27 +298,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>TPS:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>where the Expected Load:</t>
+      <t>where the Expected Capacity Load:</t>
     </r>
     <r>
       <rPr>
@@ -264,82 +312,7 @@
     </r>
   </si>
   <si>
-    <t>16 min</t>
-  </si>
-  <si>
-    <t>15 min</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">Load Test </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="7"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">Fail </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>TPS:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>1.984</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>where The Expected Load:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>2.778</t>
-    </r>
+    <t>Capacity point</t>
   </si>
 </sst>
 </file>
@@ -440,12 +413,6 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="0"/>
-      <name val="Arial Rounded MT Bold"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="7" tint="0.59999389629810485"/>
@@ -480,17 +447,22 @@
       <family val="3"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="6"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Arial Rounded MT Bold"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="0"/>
+      <name val="Arial Rounded MT Bold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="16">
@@ -585,7 +557,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -608,12 +580,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -702,7 +683,6 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -718,22 +698,27 @@
     <xf numFmtId="10" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,8 +1010,8 @@
   </sheetPr>
   <dimension ref="B4:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G16" sqref="D16:G16"/>
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1181,7 @@
       <c r="F13" s="29">
         <v>1667</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="34">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
@@ -1214,7 +1199,7 @@
       <c r="F14" s="21">
         <v>1667</v>
       </c>
-      <c r="G14" s="35">
+      <c r="G14" s="34">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
@@ -1232,7 +1217,7 @@
       <c r="F15" s="21">
         <v>1667</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G15" s="34">
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
@@ -1250,10 +1235,10 @@
       <c r="F16" s="21">
         <v>1667</v>
       </c>
-      <c r="G16" s="40">
+      <c r="G16" s="37">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="38" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1261,7 +1246,7 @@
       <c r="B17" s="19"/>
       <c r="C17" s="20"/>
       <c r="D17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="21">
         <v>900</v>
@@ -1269,7 +1254,7 @@
       <c r="F17" s="21">
         <v>1667</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="37">
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
@@ -1279,7 +1264,7 @@
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="21">
         <v>960</v>
@@ -1287,7 +1272,7 @@
       <c r="F18" s="21">
         <v>1667</v>
       </c>
-      <c r="G18" s="35">
+      <c r="G18" s="34">
         <v>1.8E-3</v>
       </c>
     </row>
@@ -1305,7 +1290,7 @@
       <c r="F19" s="21">
         <v>1667</v>
       </c>
-      <c r="G19" s="35">
+      <c r="G19" s="34">
         <v>1E-3</v>
       </c>
     </row>
@@ -1322,14 +1307,14 @@
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="2:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
+      <c r="B21" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1348,10 +1333,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,20 +1345,20 @@
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+    <row r="2" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1383,7 +1368,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1403,7 +1388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
@@ -1421,7 +1406,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
@@ -1439,7 +1424,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
@@ -1453,7 +1438,7 @@
       </c>
       <c r="G7" s="24"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
         <v>25</v>
       </c>
@@ -1467,11 +1452,17 @@
       <c r="F8" s="21">
         <v>1667</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="33">
         <v>2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="42">
+        <v>1.984</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>26</v>
       </c>
@@ -1483,20 +1474,27 @@
         <v>840</v>
       </c>
       <c r="F9" s="21">
-        <v>3000</v>
-      </c>
-      <c r="G9" s="34"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+        <v>2000</v>
+      </c>
+      <c r="G9" s="33">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
-      <c r="G10" s="34"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="21">
+        <v>4000</v>
+      </c>
+      <c r="G10" s="33">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
         <v>28</v>
       </c>
@@ -1507,37 +1505,40 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
-      <c r="G12" s="33"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="43" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="42">
+        <v>1.984</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="20"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
       <c r="C15" s="20"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
@@ -1545,7 +1546,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
       <c r="C17" s="20"/>
       <c r="D17" s="21"/>
@@ -1553,7 +1554,7 @@
       <c r="F17" s="21"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
       <c r="C18" s="20"/>
       <c r="D18" s="21"/>
@@ -1561,7 +1562,7 @@
       <c r="F18" s="21"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
@@ -1569,14 +1570,14 @@
       <c r="F19" s="21"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
         <v>5</v>
       </c>
@@ -1586,21 +1587,22 @@
       <c r="F21" s="25"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="2:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
+    <row r="22" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B22:H22"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1694,7 +1696,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="21">
         <v>960</v>
@@ -1702,7 +1704,7 @@
       <c r="D12" s="21">
         <v>1667</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="34">
         <v>1.8E-3</v>
       </c>
     </row>
@@ -1716,7 +1718,7 @@
       <c r="D13" s="21">
         <v>1667</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="34">
         <v>8.0000000000000004E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
report SS not showing issue fixed
</commit_message>
<xml_diff>
--- a/booking-API-Load_Stress-TestReport.xlsx
+++ b/booking-API-Load_Stress-TestReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\temmm\Full stack SQA_Road to SDET\assinmt\3 Load test using Jmeter\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCDAD60-36E1-43BB-81C0-A1C2DAF8B575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B5E3DA-68B8-496B-9BF4-AE788CDC8F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="825" windowWidth="18300" windowHeight="9255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Load-Test-Report" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Test Name</t>
   </si>
@@ -105,9 +105,6 @@
     </r>
   </si>
   <si>
-    <t>Capacity Point</t>
-  </si>
-  <si>
     <t>Lower Bottleneck</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>20 min</t>
   </si>
   <si>
-    <t>Test-9</t>
-  </si>
-  <si>
     <t>Test Step-1</t>
   </si>
   <si>
@@ -186,6 +180,64 @@
   </si>
   <si>
     <t>15 min</t>
+  </si>
+  <si>
+    <t>Capacity point</t>
+  </si>
+  <si>
+    <t>Test Step-10</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Stress Test</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Lower Bottleneck: 7.738 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">although the Expected </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">Capacity Load:2.778 </t>
+    </r>
   </si>
   <si>
     <r>
@@ -206,7 +258,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve">Fail </t>
+      <t xml:space="preserve">Fail. </t>
     </r>
     <r>
       <rPr>
@@ -246,7 +298,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>where The Expected Load:</t>
+      <t>although the Expected Load:</t>
     </r>
     <r>
       <rPr>
@@ -259,67 +311,12 @@
       <t>2.778</t>
     </r>
   </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Stress Test</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="7" tint="0.59999389629810485"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">Lower Bottleneck: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>where the Expected Capacity Load:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">2.778 </t>
-    </r>
-  </si>
-  <si>
-    <t>Capacity point</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,12 +442,6 @@
       <color theme="7" tint="0.59999389629810485"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color theme="0" tint="-0.34998626667073579"/>
-      <name val="Arial Rounded MT Bold"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="7"/>
@@ -510,6 +501,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -550,14 +547,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor rgb="FF93C47D"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -584,6 +575,17 @@
       <left style="thin">
         <color theme="0" tint="-4.9989318521683403E-2"/>
       </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -594,8 +596,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="13" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="13" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,117 +703,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="13" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,10 +1010,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="B4:H21"/>
+  <dimension ref="B4:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,301 +1022,307 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+    </row>
+    <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="12">
         <v>12</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="12">
         <v>720</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="13">
         <v>43200</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="13">
         <v>120000</v>
       </c>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="3">
         <v>60</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="3">
         <v>3600</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="4">
         <v>10000</v>
       </c>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="23">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="18">
         <v>1</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="19">
         <v>2.778</v>
       </c>
-      <c r="G9" s="24"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+      <c r="G9" s="19"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="16">
+        <v>60</v>
+      </c>
+      <c r="F10" s="16">
+        <v>167</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="16">
+        <v>300</v>
+      </c>
+      <c r="F11" s="16">
+        <v>833</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="21">
-        <v>60</v>
-      </c>
-      <c r="F10" s="21">
-        <v>167</v>
-      </c>
-      <c r="G10" s="12">
+      <c r="C12" s="15"/>
+      <c r="D12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="16">
+        <v>540</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1500</v>
+      </c>
+      <c r="G12" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="21">
-        <v>300</v>
-      </c>
-      <c r="F11" s="21">
-        <v>833</v>
-      </c>
-      <c r="G11" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="24">
+        <v>600</v>
+      </c>
+      <c r="F13" s="24">
+        <v>1667</v>
+      </c>
+      <c r="G13" s="25">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="16">
+        <v>660</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1667</v>
+      </c>
+      <c r="G14" s="25">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="16">
+        <v>720</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1667</v>
+      </c>
+      <c r="G15" s="25">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="21">
-        <v>540</v>
-      </c>
-      <c r="F12" s="21">
-        <v>1500</v>
-      </c>
-      <c r="G12" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="29">
-        <v>600</v>
-      </c>
-      <c r="F13" s="29">
+      <c r="E16" s="16">
+        <v>840</v>
+      </c>
+      <c r="F16" s="16">
         <v>1667</v>
       </c>
-      <c r="G13" s="34">
-        <v>1.1999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="21">
-        <v>660</v>
-      </c>
-      <c r="F14" s="21">
+      <c r="G16" s="27">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="28">
+        <v>1.984</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="16">
+        <v>900</v>
+      </c>
+      <c r="F17" s="16">
         <v>1667</v>
       </c>
-      <c r="G14" s="34">
-        <v>5.9999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="21">
-        <v>720</v>
-      </c>
-      <c r="F15" s="21">
+      <c r="G17" s="27">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="16">
+        <v>960</v>
+      </c>
+      <c r="F18" s="16">
         <v>1667</v>
       </c>
-      <c r="G15" s="34">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="21">
-        <v>840</v>
-      </c>
-      <c r="F16" s="21">
+      <c r="G18" s="25">
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1200</v>
+      </c>
+      <c r="F19" s="16">
         <v>1667</v>
       </c>
-      <c r="G16" s="37">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="H16" s="38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="21">
-        <v>900</v>
-      </c>
-      <c r="F17" s="21">
-        <v>1667</v>
-      </c>
-      <c r="G17" s="37">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="21">
-        <v>960</v>
-      </c>
-      <c r="F18" s="21">
-        <v>1667</v>
-      </c>
-      <c r="G18" s="34">
-        <v>1.8E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="21">
-        <v>1200</v>
-      </c>
-      <c r="F19" s="21">
-        <v>1667</v>
-      </c>
-      <c r="G19" s="34">
+      <c r="G19" s="25">
         <v>1E-3</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="25">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="20">
         <v>1.984</v>
       </c>
-      <c r="G20" s="15"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" spans="2:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
+      <c r="B21" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1333,10 +1341,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B2:I22"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,264 +1353,279 @@
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="B2" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="12">
         <v>12</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="12">
         <v>720</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="13">
         <v>43200</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="13">
         <v>120000</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="3">
         <v>60</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="3">
         <v>3600</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="4">
         <v>10000</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="23">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="18">
         <v>1</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="19">
         <v>2.778</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="16">
+        <v>840</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1667</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="16">
+        <v>840</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2000</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="21">
+      <c r="C10" s="15"/>
+      <c r="D10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="16">
         <v>840</v>
       </c>
-      <c r="F8" s="21">
-        <v>1667</v>
-      </c>
-      <c r="G8" s="33">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="H8" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="42">
-        <v>1.984</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="F10" s="16">
+        <v>3000</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="21">
+      <c r="C11" s="15"/>
+      <c r="D11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="16">
         <v>840</v>
       </c>
-      <c r="F9" s="21">
-        <v>2000</v>
-      </c>
-      <c r="G9" s="33">
-        <v>2.2000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+      <c r="F11" s="16">
+        <v>5000</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21">
-        <v>4000</v>
-      </c>
-      <c r="G10" s="33">
-        <v>5.9999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="16">
+        <v>840</v>
+      </c>
+      <c r="F12" s="16">
+        <v>6500</v>
+      </c>
+      <c r="G12" s="7">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="28">
+        <v>7.7380000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="16">
+        <v>840</v>
+      </c>
+      <c r="F13" s="16">
+        <v>7000</v>
+      </c>
+      <c r="G13" s="7">
+        <v>6.4500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="42">
-        <v>1.984</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="16">
+        <v>840</v>
+      </c>
+      <c r="F14" s="16">
+        <v>7500</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0.25119999999999998</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="16">
+        <v>840</v>
+      </c>
+      <c r="F15" s="26">
+        <v>10000</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.52100000000000002</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="26" t="s">
+      <c r="B16" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="19">
+        <v>7.7380000000000004</v>
+      </c>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1621,104 +1644,104 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="16">
+        <v>660</v>
+      </c>
+      <c r="D7" s="16">
+        <v>1667</v>
+      </c>
+      <c r="E7" s="17">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="C8" s="16">
+        <v>720</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1667</v>
+      </c>
+      <c r="E8" s="17">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="22">
+        <v>14</v>
+      </c>
+      <c r="C9" s="22">
+        <v>840</v>
+      </c>
+      <c r="D9" s="22">
+        <v>1667</v>
+      </c>
+      <c r="E9" s="23">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="22">
+        <v>15</v>
+      </c>
+      <c r="C10" s="22">
+        <v>900</v>
+      </c>
+      <c r="D10" s="22">
+        <v>1667</v>
+      </c>
+      <c r="E10" s="23">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="22">
         <v>16</v>
       </c>
-      <c r="C7" s="21">
-        <v>660</v>
-      </c>
-      <c r="D7" s="21">
+      <c r="C11" s="22">
+        <v>960</v>
+      </c>
+      <c r="D11" s="22">
         <v>1667</v>
       </c>
-      <c r="E7" s="22">
-        <v>5.9999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="21">
-        <v>720</v>
-      </c>
-      <c r="D8" s="21">
+      <c r="E11" s="23">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="16">
+        <v>960</v>
+      </c>
+      <c r="D12" s="16">
         <v>1667</v>
       </c>
-      <c r="E8" s="22">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="27">
-        <v>14</v>
-      </c>
-      <c r="C9" s="27">
-        <v>840</v>
-      </c>
-      <c r="D9" s="27">
+      <c r="E12" s="25">
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="16">
+        <v>1200</v>
+      </c>
+      <c r="D13" s="16">
         <v>1667</v>
       </c>
-      <c r="E9" s="28">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="27">
-        <v>15</v>
-      </c>
-      <c r="C10" s="27">
-        <v>900</v>
-      </c>
-      <c r="D10" s="27">
-        <v>1667</v>
-      </c>
-      <c r="E10" s="28">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="27">
-        <v>16</v>
-      </c>
-      <c r="C11" s="27">
-        <v>960</v>
-      </c>
-      <c r="D11" s="27">
-        <v>1667</v>
-      </c>
-      <c r="E11" s="28">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="21">
-        <v>960</v>
-      </c>
-      <c r="D12" s="21">
-        <v>1667</v>
-      </c>
-      <c r="E12" s="34">
-        <v>1.8E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="21">
-        <v>1200</v>
-      </c>
-      <c r="D13" s="21">
-        <v>1667</v>
-      </c>
-      <c r="E13" s="34">
+      <c r="E13" s="25">
         <v>8.0000000000000004E-4</v>
       </c>
     </row>

</xml_diff>